<commit_message>
added trivial_difference() - there are problems with duplicates
</commit_message>
<xml_diff>
--- a/new receipts of DSO/new receipts of DSO 2022-08-24.xlsx
+++ b/new receipts of DSO/new receipts of DSO 2022-08-24.xlsx
@@ -7,14 +7,14 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="2022-08-24" sheetId="1" r:id="rId1"/>
+    <sheet name="New as of 2022-08-24" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="19">
   <si>
     <t>Обозначение документа</t>
   </si>
@@ -432,7 +432,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G7"/>
+  <dimension ref="A1:G9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
@@ -552,10 +552,13 @@
     </row>
     <row r="6" spans="1:7">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>9</v>
+      </c>
+      <c r="B6">
+        <v>7</v>
       </c>
       <c r="C6" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="D6" t="s">
         <v>17</v>
@@ -564,27 +567,64 @@
         <v>18</v>
       </c>
       <c r="F6" s="2">
-        <v>44271</v>
+        <v>44692</v>
       </c>
     </row>
     <row r="7" spans="1:7">
       <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F7" s="2">
+        <v>44271</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" t="s">
         <v>11</v>
       </c>
-      <c r="B7">
+      <c r="B8">
         <v>4</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C8" t="s">
         <v>16</v>
       </c>
-      <c r="D7" t="s">
-        <v>17</v>
-      </c>
-      <c r="E7" t="s">
-        <v>18</v>
-      </c>
-      <c r="F7" s="2">
+      <c r="D8" t="s">
+        <v>17</v>
+      </c>
+      <c r="E8" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="2">
         <v>44692</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7">
+      <c r="A9" t="s">
+        <v>11</v>
+      </c>
+      <c r="B9">
+        <v>5</v>
+      </c>
+      <c r="C9" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" t="s">
+        <v>17</v>
+      </c>
+      <c r="E9" t="s">
+        <v>18</v>
+      </c>
+      <c r="F9" s="2">
+        <v>44042</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
added find_identical_cells() - and merging cells
</commit_message>
<xml_diff>
--- a/new receipts of DSO/new receipts of DSO 2022-08-24.xlsx
+++ b/new receipts of DSO/new receipts of DSO 2022-08-24.xlsx
@@ -7,70 +7,291 @@
     <workbookView xWindow="240" yWindow="15" windowWidth="16095" windowHeight="9660"/>
   </bookViews>
   <sheets>
-    <sheet name="New as of 2022-08-24" sheetId="1" r:id="rId1"/>
+    <sheet name="New as of 2022-08-25" sheetId="1" r:id="rId1"/>
   </sheets>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="16">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="172" uniqueCount="90">
+  <si>
+    <t>Город</t>
+  </si>
+  <si>
+    <t>Организация</t>
+  </si>
   <si>
     <t>Обозначение документа</t>
   </si>
   <si>
-    <t>№  изм.</t>
-  </si>
-  <si>
     <t>Наименование</t>
   </si>
   <si>
-    <t>Город</t>
-  </si>
-  <si>
-    <t>Организация</t>
-  </si>
-  <si>
-    <t>Дата ввода информации (фильтр новых поступлений)</t>
-  </si>
-  <si>
-    <t>Примечание</t>
-  </si>
-  <si>
-    <t>АБВГ.123456.001 СБ</t>
-  </si>
-  <si>
-    <t>АБВГ.123456.009</t>
-  </si>
-  <si>
-    <t>АБВГ.123456.010</t>
-  </si>
-  <si>
-    <t>10</t>
+    <t>Самара</t>
+  </si>
+  <si>
+    <t>Миасс</t>
+  </si>
+  <si>
+    <t>Москва</t>
+  </si>
+  <si>
+    <t>Каменск-Уральский</t>
+  </si>
+  <si>
+    <t>Санкт-Петербург</t>
+  </si>
+  <si>
+    <t>АО «РКЦ «Прогресс»</t>
+  </si>
+  <si>
+    <t>АО «ГРЦ Макеева»</t>
+  </si>
+  <si>
+    <t>АО «Корпорация «МИТ»</t>
+  </si>
+  <si>
+    <t>АО «УПКБ «Деталь»</t>
+  </si>
+  <si>
+    <t>АО "Концерн "ЦНИИ "Электроприбор"</t>
+  </si>
+  <si>
+    <t>АО «НИИ Командных приборов»</t>
+  </si>
+  <si>
+    <t>НИИСИ РАН</t>
+  </si>
+  <si>
+    <t>14А15 ИЭ60   Издание первое</t>
+  </si>
+  <si>
+    <t xml:space="preserve">14А15.БВВ-РНС2.0000-0РР02
+</t>
+  </si>
+  <si>
+    <t>14с748 ИЭ17 часть 1
+Издание первое</t>
+  </si>
+  <si>
+    <t>14С748.0000-0Э6-23</t>
+  </si>
+  <si>
+    <t>15А28.П.55.25.002</t>
+  </si>
+  <si>
+    <t>15А28.П.55.25.101</t>
+  </si>
+  <si>
+    <t>15А28.Р.51.10.080 Э3</t>
+  </si>
+  <si>
+    <t>15А28.Р.51.10.240 Э3</t>
+  </si>
+  <si>
+    <t>374СА11.02.07.000</t>
+  </si>
+  <si>
+    <t>374СА11.02.07.000  СБ</t>
+  </si>
+  <si>
+    <t>374СА11.02.07.100</t>
+  </si>
+  <si>
+    <t>374СА11.02.07.100  СБ</t>
+  </si>
+  <si>
+    <t>374СА11.02.07.210 СБ</t>
+  </si>
+  <si>
+    <t>3Л-30.30.00.000 СБ</t>
+  </si>
+  <si>
+    <t>3Л-30.30.00.100 СБ</t>
+  </si>
+  <si>
+    <t>ГУ8.229.022</t>
+  </si>
+  <si>
+    <t>ДНИЯ.294709.018 (с входящими)</t>
+  </si>
+  <si>
+    <t>ДНИЯ.296361.004</t>
+  </si>
+  <si>
+    <t>ДНИЯ.296361.004 СБ</t>
+  </si>
+  <si>
+    <t>ДНИЯ.301568.021</t>
+  </si>
+  <si>
+    <t>ДНИЯ.301568.021 СБ</t>
+  </si>
+  <si>
+    <t>ДНИЯ.304274.030</t>
+  </si>
+  <si>
+    <t>ДНИЯ.304274.030 СБ</t>
+  </si>
+  <si>
+    <t>ДНИЯ.711147.157</t>
+  </si>
+  <si>
+    <t>ДНИЯ.711171.067</t>
+  </si>
+  <si>
+    <t>ДНИЯ.713362.028</t>
+  </si>
+  <si>
+    <t>ДНИЯ.713611.013</t>
+  </si>
+  <si>
+    <t>ДНИЯ.714333.029</t>
+  </si>
+  <si>
+    <t>ДНИЯ.714533.002</t>
+  </si>
+  <si>
+    <t>ДНИЯ.734323.021</t>
+  </si>
+  <si>
+    <t>ДНИЯ.741166.010</t>
+  </si>
+  <si>
+    <t>ДНИЯ.758128.005</t>
+  </si>
+  <si>
+    <t>ДНИЯ.758151.211</t>
+  </si>
+  <si>
+    <t>ДНИЯ.766167.001</t>
+  </si>
+  <si>
+    <t>ИНАЯ.402113.130 И27</t>
+  </si>
+  <si>
+    <t>ИНАЯ.402113.130 И36</t>
+  </si>
+  <si>
+    <t>ЛРДА.90144-01 13 01</t>
+  </si>
+  <si>
+    <t>МАВИ.713511.007</t>
+  </si>
+  <si>
+    <t>НИДБ.461545.001 И3</t>
+  </si>
+  <si>
+    <t>НИДБ.461545.001 ИЭ10</t>
+  </si>
+  <si>
+    <t>НИДБ.461545.001 ИЭ12</t>
+  </si>
+  <si>
+    <t>Инструкция по подготовке данных на пуск(14А14 ИЭ60). Издание первое (с 1 изделия)</t>
+  </si>
+  <si>
+    <t>РКН 14А15.БВВ-РНС2  Расчет  баллистический</t>
+  </si>
+  <si>
+    <t>Изделие  14С748 Инструкция  по  электрическим проверкам</t>
+  </si>
+  <si>
+    <t>Сборочно-защитный  блок. Транзитный кабель и кабели СУ</t>
+  </si>
+  <si>
+    <t>Скоба2</t>
+  </si>
+  <si>
+    <t>Задвижка</t>
+  </si>
+  <si>
+    <t>Сборка кабельная К308</t>
+  </si>
+  <si>
+    <t>Сборка кабельная 394</t>
+  </si>
+  <si>
+    <t>Блок датчиков давления</t>
+  </si>
+  <si>
+    <t>Заборн  R</t>
+  </si>
+  <si>
+    <t>Заборник</t>
+  </si>
+  <si>
+    <t>Корпус   с  втулкой</t>
+  </si>
+  <si>
+    <t>Корпус ПрО</t>
   </si>
   <si>
     <t>Корпус</t>
   </si>
   <si>
-    <t>Крышка нижняя</t>
-  </si>
-  <si>
-    <t>Крышка</t>
-  </si>
-  <si>
-    <t>Хоторн</t>
-  </si>
-  <si>
-    <t>SpaceX</t>
+    <t>Втулка</t>
+  </si>
+  <si>
+    <t>Комплект приспособлений и инструмента для штифтовки</t>
+  </si>
+  <si>
+    <t>Приспособление для штифтовки</t>
+  </si>
+  <si>
+    <t>Кронштейн</t>
+  </si>
+  <si>
+    <t>Упор</t>
+  </si>
+  <si>
+    <t>Кольцо</t>
+  </si>
+  <si>
+    <t>Гильза</t>
+  </si>
+  <si>
+    <t>Обойма</t>
+  </si>
+  <si>
+    <t>Стойка</t>
+  </si>
+  <si>
+    <t>Болт</t>
+  </si>
+  <si>
+    <t>Винт</t>
+  </si>
+  <si>
+    <t>Валик контрольный</t>
+  </si>
+  <si>
+    <t>Комплекс командных приборов. Инструкция по внешнему осмотру</t>
+  </si>
+  <si>
+    <t>Комплекс командных приборов. Инструкция по оценке параметров системы телеметрических измерений</t>
+  </si>
+  <si>
+    <t>Программный продукт</t>
+  </si>
+  <si>
+    <t>Стержень</t>
+  </si>
+  <si>
+    <t>ИПК. Инструкция по проверке</t>
+  </si>
+  <si>
+    <t>ИПК. Инструкция по монтажу кабельного комплекта</t>
+  </si>
+  <si>
+    <t>ИПК. Инструкция по определению АБН при монтаже и периодическом РТО</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <numFmts count="1">
-    <numFmt numFmtId="164" formatCode="YYYY-MM-DD HH:MM:SS"/>
-  </numFmts>
   <fonts count="2">
     <font>
       <sz val="11"/>
@@ -81,11 +302,10 @@
     </font>
     <font>
       <b/>
-      <sz val="11"/>
+      <sz val="14"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Times New Roman"/>
       <family val="2"/>
-      <scheme val="minor"/>
     </font>
   </fonts>
   <fills count="2">
@@ -123,12 +343,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="top"/>
+      <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -423,22 +642,20 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:G4"/>
+  <dimension ref="A1:D42"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="26.7109375" customWidth="1"/>
-    <col min="2" max="2" width="12.7109375" customWidth="1"/>
-    <col min="3" max="3" width="18.7109375" customWidth="1"/>
-    <col min="4" max="4" width="11.7109375" customWidth="1"/>
-    <col min="5" max="5" width="16.7109375" customWidth="1"/>
-    <col min="6" max="6" width="53.7109375" customWidth="1"/>
-    <col min="7" max="7" width="15.7109375" customWidth="1"/>
+    <col min="1" max="1" width="21.7109375" customWidth="1"/>
+    <col min="2" max="2" width="37.7109375" customWidth="1"/>
+    <col min="3" max="3" width="38.7109375" customWidth="1"/>
+    <col min="4" max="4" width="98.7109375" customWidth="1"/>
+    <col min="6" max="6" width="15.7109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7">
+    <row r="1" spans="1:4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -451,71 +668,579 @@
       <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="1" t="s">
+    </row>
+    <row r="2" spans="1:4">
+      <c r="A2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="B2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D2" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4">
+      <c r="A3" t="s">
+        <v>4</v>
+      </c>
+      <c r="B3" t="s">
+        <v>9</v>
+      </c>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" t="s">
+        <v>18</v>
+      </c>
+      <c r="D4" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4">
+      <c r="A5" t="s">
+        <v>4</v>
+      </c>
+      <c r="B5" t="s">
+        <v>9</v>
+      </c>
+      <c r="C5" t="s">
+        <v>19</v>
+      </c>
+      <c r="D5" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4">
+      <c r="A6" t="s">
         <v>5</v>
       </c>
-      <c r="G1" s="1" t="s">
+      <c r="B6" t="s">
+        <v>10</v>
+      </c>
+      <c r="C6" t="s">
+        <v>20</v>
+      </c>
+      <c r="D6" t="s">
+        <v>61</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
+        <v>10</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>62</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4">
+      <c r="A8" t="s">
+        <v>5</v>
+      </c>
+      <c r="B8" t="s">
+        <v>10</v>
+      </c>
+      <c r="C8" t="s">
+        <v>22</v>
+      </c>
+      <c r="D8" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4">
+      <c r="A9" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" t="s">
+        <v>10</v>
+      </c>
+      <c r="C9" t="s">
+        <v>23</v>
+      </c>
+      <c r="D9" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4">
+      <c r="A10" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="2" spans="1:7">
-      <c r="A2" t="s">
+      <c r="B10" t="s">
+        <v>11</v>
+      </c>
+      <c r="C10" t="s">
+        <v>24</v>
+      </c>
+      <c r="D10" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4">
+      <c r="A11" t="s">
+        <v>6</v>
+      </c>
+      <c r="B11" t="s">
+        <v>11</v>
+      </c>
+      <c r="C11" t="s">
+        <v>25</v>
+      </c>
+      <c r="D11" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4">
+      <c r="A12" t="s">
+        <v>6</v>
+      </c>
+      <c r="B12" t="s">
+        <v>11</v>
+      </c>
+      <c r="C12" t="s">
+        <v>26</v>
+      </c>
+      <c r="D12" t="s">
+        <v>66</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4">
+      <c r="A13" t="s">
+        <v>6</v>
+      </c>
+      <c r="B13" t="s">
+        <v>11</v>
+      </c>
+      <c r="C13" t="s">
+        <v>27</v>
+      </c>
+      <c r="D13" t="s">
+        <v>67</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4">
+      <c r="A14" t="s">
+        <v>6</v>
+      </c>
+      <c r="B14" t="s">
+        <v>11</v>
+      </c>
+      <c r="C14" t="s">
+        <v>28</v>
+      </c>
+      <c r="D14" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4">
+      <c r="A15" t="s">
+        <v>6</v>
+      </c>
+      <c r="B15" t="s">
+        <v>11</v>
+      </c>
+      <c r="C15" t="s">
+        <v>29</v>
+      </c>
+      <c r="D15" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4">
+      <c r="A16" t="s">
+        <v>6</v>
+      </c>
+      <c r="B16" t="s">
+        <v>11</v>
+      </c>
+      <c r="C16" t="s">
+        <v>30</v>
+      </c>
+      <c r="D16" t="s">
+        <v>70</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4">
+      <c r="A17" t="s">
         <v>7</v>
       </c>
-      <c r="B2" t="s">
-        <v>10</v>
-      </c>
-      <c r="C2" t="s">
-        <v>11</v>
-      </c>
-      <c r="D2" t="s">
+      <c r="B17" t="s">
+        <v>12</v>
+      </c>
+      <c r="C17" t="s">
+        <v>31</v>
+      </c>
+      <c r="D17" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4">
+      <c r="A18" t="s">
+        <v>8</v>
+      </c>
+      <c r="B18" t="s">
+        <v>13</v>
+      </c>
+      <c r="C18" t="s">
+        <v>32</v>
+      </c>
+      <c r="D18" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4">
+      <c r="A19" t="s">
+        <v>8</v>
+      </c>
+      <c r="B19" t="s">
+        <v>13</v>
+      </c>
+      <c r="C19" t="s">
+        <v>33</v>
+      </c>
+      <c r="D19" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4">
+      <c r="A20" t="s">
+        <v>8</v>
+      </c>
+      <c r="B20" t="s">
+        <v>13</v>
+      </c>
+      <c r="C20" t="s">
+        <v>34</v>
+      </c>
+      <c r="D20" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4">
+      <c r="A21" t="s">
+        <v>8</v>
+      </c>
+      <c r="B21" t="s">
+        <v>13</v>
+      </c>
+      <c r="C21" t="s">
+        <v>35</v>
+      </c>
+      <c r="D21" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4">
+      <c r="A22" t="s">
+        <v>8</v>
+      </c>
+      <c r="B22" t="s">
+        <v>13</v>
+      </c>
+      <c r="C22" t="s">
+        <v>36</v>
+      </c>
+      <c r="D22" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4">
+      <c r="A23" t="s">
+        <v>8</v>
+      </c>
+      <c r="B23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C23" t="s">
+        <v>37</v>
+      </c>
+      <c r="D23" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4">
+      <c r="A24" t="s">
+        <v>8</v>
+      </c>
+      <c r="B24" t="s">
+        <v>13</v>
+      </c>
+      <c r="C24" t="s">
+        <v>38</v>
+      </c>
+      <c r="D24" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4">
+      <c r="A25" t="s">
+        <v>8</v>
+      </c>
+      <c r="B25" t="s">
+        <v>13</v>
+      </c>
+      <c r="C25" t="s">
+        <v>39</v>
+      </c>
+      <c r="D25" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4">
+      <c r="A26" t="s">
+        <v>8</v>
+      </c>
+      <c r="B26" t="s">
+        <v>13</v>
+      </c>
+      <c r="C26" t="s">
+        <v>40</v>
+      </c>
+      <c r="D26" t="s">
+        <v>76</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4">
+      <c r="A27" t="s">
+        <v>8</v>
+      </c>
+      <c r="B27" t="s">
+        <v>13</v>
+      </c>
+      <c r="C27" t="s">
+        <v>41</v>
+      </c>
+      <c r="D27" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4">
+      <c r="A28" t="s">
+        <v>8</v>
+      </c>
+      <c r="B28" t="s">
+        <v>13</v>
+      </c>
+      <c r="C28" t="s">
+        <v>42</v>
+      </c>
+      <c r="D28" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4">
+      <c r="A29" t="s">
+        <v>8</v>
+      </c>
+      <c r="B29" t="s">
+        <v>13</v>
+      </c>
+      <c r="C29" t="s">
+        <v>43</v>
+      </c>
+      <c r="D29" t="s">
+        <v>77</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4">
+      <c r="A30" t="s">
+        <v>8</v>
+      </c>
+      <c r="B30" t="s">
+        <v>13</v>
+      </c>
+      <c r="C30" t="s">
+        <v>44</v>
+      </c>
+      <c r="D30" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4">
+      <c r="A31" t="s">
+        <v>8</v>
+      </c>
+      <c r="B31" t="s">
+        <v>13</v>
+      </c>
+      <c r="C31" t="s">
+        <v>45</v>
+      </c>
+      <c r="D31" t="s">
+        <v>74</v>
+      </c>
+    </row>
+    <row r="32" spans="1:4">
+      <c r="A32" t="s">
+        <v>8</v>
+      </c>
+      <c r="B32" t="s">
+        <v>13</v>
+      </c>
+      <c r="C32" t="s">
+        <v>46</v>
+      </c>
+      <c r="D32" t="s">
+        <v>79</v>
+      </c>
+    </row>
+    <row r="33" spans="1:4">
+      <c r="A33" t="s">
+        <v>8</v>
+      </c>
+      <c r="B33" t="s">
+        <v>13</v>
+      </c>
+      <c r="C33" t="s">
+        <v>47</v>
+      </c>
+      <c r="D33" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="34" spans="1:4">
+      <c r="A34" t="s">
+        <v>8</v>
+      </c>
+      <c r="B34" t="s">
+        <v>13</v>
+      </c>
+      <c r="C34" t="s">
+        <v>48</v>
+      </c>
+      <c r="D34" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="35" spans="1:4">
+      <c r="A35" t="s">
+        <v>8</v>
+      </c>
+      <c r="B35" t="s">
+        <v>13</v>
+      </c>
+      <c r="C35" t="s">
+        <v>49</v>
+      </c>
+      <c r="D35" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="36" spans="1:4">
+      <c r="A36" t="s">
+        <v>8</v>
+      </c>
+      <c r="B36" t="s">
         <v>14</v>
       </c>
-      <c r="E2" t="s">
+      <c r="C36" t="s">
+        <v>50</v>
+      </c>
+      <c r="D36" t="s">
+        <v>83</v>
+      </c>
+    </row>
+    <row r="37" spans="1:4">
+      <c r="A37" t="s">
+        <v>8</v>
+      </c>
+      <c r="B37" t="s">
+        <v>14</v>
+      </c>
+      <c r="C37" t="s">
+        <v>51</v>
+      </c>
+      <c r="D37" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="38" spans="1:4">
+      <c r="A38" t="s">
+        <v>6</v>
+      </c>
+      <c r="B38" t="s">
         <v>15</v>
       </c>
-      <c r="F2" s="2">
-        <v>44692</v>
-      </c>
-    </row>
-    <row r="3" spans="1:7">
-      <c r="A3" t="s">
-        <v>8</v>
-      </c>
-      <c r="B3">
+      <c r="C38" t="s">
+        <v>52</v>
+      </c>
+      <c r="D38" t="s">
+        <v>85</v>
+      </c>
+    </row>
+    <row r="39" spans="1:4">
+      <c r="A39" t="s">
         <v>7</v>
       </c>
-      <c r="C3" t="s">
+      <c r="B39" t="s">
         <v>12</v>
       </c>
-      <c r="D3" t="s">
-        <v>14</v>
-      </c>
-      <c r="E3" t="s">
-        <v>15</v>
-      </c>
-      <c r="F3" s="2">
-        <v>44692</v>
-      </c>
-    </row>
-    <row r="4" spans="1:7">
-      <c r="A4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>13</v>
-      </c>
-      <c r="D4" t="s">
-        <v>14</v>
-      </c>
-      <c r="E4" t="s">
-        <v>15</v>
-      </c>
-      <c r="F4" s="2">
-        <v>44271</v>
+      <c r="C39" t="s">
+        <v>53</v>
+      </c>
+      <c r="D39" t="s">
+        <v>86</v>
+      </c>
+    </row>
+    <row r="40" spans="1:4">
+      <c r="A40" t="s">
+        <v>8</v>
+      </c>
+      <c r="B40" t="s">
+        <v>13</v>
+      </c>
+      <c r="C40" t="s">
+        <v>54</v>
+      </c>
+      <c r="D40" t="s">
+        <v>87</v>
+      </c>
+    </row>
+    <row r="41" spans="1:4">
+      <c r="A41" t="s">
+        <v>8</v>
+      </c>
+      <c r="B41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C41" t="s">
+        <v>55</v>
+      </c>
+      <c r="D41" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="42" spans="1:4">
+      <c r="A42" t="s">
+        <v>8</v>
+      </c>
+      <c r="B42" t="s">
+        <v>13</v>
+      </c>
+      <c r="C42" t="s">
+        <v>56</v>
+      </c>
+      <c r="D42" t="s">
+        <v>89</v>
       </c>
     </row>
   </sheetData>

</xml_diff>